<commit_message>
Automatische test-sync: 2025-06-29 13:52:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -721,8 +721,60 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #2: Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Helaas kan ik geen bestellingen plaatsen, maar ik kan u doorverwijzen naar het bestelteam binnen ons bedrijf. Graag ontvang ik de contactgegevens van uw bedrijf, zodat ik de juiste persoon met u in contact kan brengen.
+Ik zie uw reactie graag tegemoet.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-29 13:52:05</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -742,7 +794,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -750,12 +802,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -770,7 +822,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -800,6 +852,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 13:59:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -773,8 +773,58 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-29 13:59:27</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -794,7 +844,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -802,12 +852,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -849,7 +899,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:01:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,8 +823,60 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #2: Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Helaas kan ik geen bestellingen plaatsen, maar ik kan u doorverwijzen naar het bestelteam binnen ons bedrijf. Graag ontvang ik de contactgegevens van uw bedrijf, zodat ik de juiste persoon met u in contact kan brengen.
+Ik zie uw reactie graag tegemoet.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:01:39</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -844,7 +896,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -852,12 +904,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -909,7 +961,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -875,8 +875,59 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #3: Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Dank u voor uw interesse in onze producten/diensten. Om u nauwkeurige informatie te verstrekken over de verzendkosten, hebben we meer details nodig zoals het product/dienst waar u naar informeert en het afleveradres. Zou u ons kunnen voorzien van deze informatie zodat we u een precieze schatting van de verzendkosten kunnen geven?
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:04:02</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -896,7 +947,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -904,12 +955,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -924,7 +975,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -964,6 +1015,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -926,8 +926,59 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Wil je dit artikel voor me inkopen?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Testmail #4: Wil je dit artikel voor me inkopen?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je interesse in ons artikel. Helaas kan ik je op basis van dit bericht niet verder helpen. Kun je meer details geven over welk artikel je wilt inkopen en op welke manier? Zo kan ik je beter assisteren.
+Met vriendelijke groet,
+[Jouw naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:06:13</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -947,7 +998,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -955,12 +1006,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1022,7 +1073,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:08:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -977,8 +977,58 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ik wil mijn bestelling annuleren</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Testmail #5: Ik wil mijn bestelling annuleren</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Om uw bestelling te annuleren, hebben we wat extra informatie nodig. Zou u zo vriendelijk willen zijn om uw bestelnummer met ons te delen? Op die manier kunnen we uw verzoek snel verwerken.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:08:25</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -998,7 +1048,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1006,12 +1056,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1026,7 +1076,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1076,6 +1126,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:10:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1027,8 +1027,59 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kun je dit intern overleggen?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Testmail #6: Kun je dit intern overleggen?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je e-mail. Kun je wat meer specifieke informatie geven over waarover je precies wilt dat er intern overlegd wordt? Op die manier kan ik ervoor zorgen dat je aanvraag bij de juiste persoon of afdeling terechtkomt.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:10:36</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1048,7 +1099,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1056,12 +1107,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1076,7 +1127,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1136,6 +1187,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1078,8 +1078,58 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:11:20</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1099,7 +1149,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1107,12 +1157,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1154,7 +1204,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:13:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1128,8 +1128,60 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Testmail #2: Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Helaas kan ik geen bestellingen plaatsen, maar ik kan u doorverwijzen naar het bestelteam binnen ons bedrijf. Graag ontvang ik de contactgegevens van uw bedrijf, zodat ik de juiste persoon met u in contact kan brengen.
+Ik zie uw reactie graag tegemoet.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:13:30</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1149,7 +1201,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1157,12 +1209,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1214,7 +1266,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1180,8 +1180,50 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Testmail #3: Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:15:40</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1201,7 +1243,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1209,12 +1251,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1276,7 +1318,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:32:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1222,8 +1222,58 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:32:40</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1243,7 +1293,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1251,12 +1301,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1298,7 +1348,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:35:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1272,8 +1272,60 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Testmail #2: Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Helaas kan ik geen bestellingen plaatsen, maar ik kan u doorverwijzen naar het bestelteam binnen ons bedrijf. Graag ontvang ik de contactgegevens van uw bedrijf, zodat ik de juiste persoon met u in contact kan brengen.
+Ik zie uw reactie graag tegemoet.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:35:08</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1293,7 +1345,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1301,12 +1353,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1358,7 +1410,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:41:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1324,8 +1324,100 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Testmail #3: Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:41:36</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wanneer zijn jullie open?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. We zijn gesloten in het weekend. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:41:40</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1345,7 +1437,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1353,12 +1445,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1400,7 +1492,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -1420,7 +1512,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1416,8 +1416,60 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Testmail #2: Kun je 10 dozen schroeven bestellen?</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Helaas kan ik geen bestellingen plaatsen, maar ik kan u doorverwijzen naar het bestelteam binnen ons bedrijf. Graag ontvang ik de contactgegevens van uw bedrijf, zodat ik de juiste persoon met u in contact kan brengen.
+Ik zie uw reactie graag tegemoet.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:43:53</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1437,7 +1489,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1445,12 +1497,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1502,7 +1554,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:46:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1468,8 +1468,50 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Testmail #3: Wat zijn de verzendkosten?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:46:04</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1489,7 +1531,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1497,12 +1539,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1564,7 +1606,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:48:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1510,8 +1510,59 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Wil je dit artikel voor me inkopen?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Testmail #4: Wil je dit artikel voor me inkopen?</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je interesse in ons artikel. Helaas kan ik je op basis van dit bericht niet verder helpen. Kun je meer details geven over welk artikel je wilt inkopen en op welke manier? Zo kan ik je beter assisteren.
+Met vriendelijke groet,
+[Jouw naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:48:22</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1531,7 +1582,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1539,12 +1590,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H19">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I19">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1582,17 +1633,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Bestelling / Levering</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Bestelling / Levering</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:51:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1561,8 +1561,58 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Ik wil mijn bestelling annuleren</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Testmail #5: Ik wil mijn bestelling annuleren</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Om uw bestelling te annuleren, hebben we wat extra informatie nodig. Zou u zo vriendelijk willen zijn om uw bestelnummer met ons te delen? Op die manier kunnen we uw verzoek snel verwerken.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:50:55</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1582,7 +1632,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1590,12 +1640,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I19">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1667,7 +1717,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:53:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1611,8 +1611,59 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Kun je dit intern overleggen?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Testmail #6: Kun je dit intern overleggen?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je e-mail. Kun je wat meer specifieke informatie geven over waarover je precies wilt dat er intern overlegd wordt? Op die manier kan ik ervoor zorgen dat je aanvraag bij de juiste persoon of afdeling terechtkomt.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:53:12</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1632,7 +1683,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1640,12 +1691,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1727,7 +1778,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:55:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1662,8 +1662,59 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Hoe kan ik iets retourneren?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Testmail #7: Hoe kan ik iets retourneren?</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Als je een artikel wilt retourneren, kun je dit doen door contact op te nemen met onze klantenservice via support@bedrijf.nl. Zij zullen je verder begeleiden bij het retourproces en eventuele vragen beantwoorden.
+Bedankt voor je begrip en medewerking.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:55:39</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1683,7 +1734,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1691,12 +1742,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1768,7 +1819,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 14:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1713,8 +1713,58 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Kun je contact opnemen met de klant?</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Testmail #8: Kun je contact opnemen met de klant?</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Beste klantenservice,
+Ik heb zojuist een testmail verstuurd (Testmail #14) om te controleren of onze klanten goed bereikbaar zijn via e-mail. Kun je bevestigen of deze testmail succesvol is ontvangen en of jullie contact hebben opgenomen met de klant?
+Met vriendelijke groet,
+[Naam]</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-06-29 14:57:51</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1734,7 +1784,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1742,12 +1792,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H22">
+  <conditionalFormatting sqref="H2:H23">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I22">
+  <conditionalFormatting sqref="I2:I23">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1762,7 +1812,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1832,6 +1882,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:00:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1763,8 +1763,58 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie voorwaarden?</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Testmail #9: Wat zijn jullie voorwaarden?</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank voor uw interesse in onze diensten. Voor informatie over onze voorwaarden kunt u terecht op onze website onder de sectie 'Algemene Voorwaarden'. Mocht u specifieke vragen hebben, dan helpen wij u graag verder. Aarzel niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:00:07</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1784,7 +1834,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G24">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1792,12 +1842,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H23">
+  <conditionalFormatting sqref="H2:H24">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I23">
+  <conditionalFormatting sqref="I2:I24">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1845,17 +1895,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:02:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1813,8 +1813,60 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Ik wil dat je dit regelt met support.</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Testmail #10: Ik wil dat je dit regelt met support.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Om uw verzoek efficiënt te kunnen afhandelen, zou ik graag wat meer informatie van u willen ontvangen. Kunt u mij alstublieft meer details geven over het specifieke probleem waarmee u hulp nodig heeft? Op die manier kunnen wij u beter van dienst zijn.
+Met vriendelijke groet,
+[Naam]  
+E-mailassistent  
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:02:17</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1834,7 +1886,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1842,12 +1894,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H24">
+  <conditionalFormatting sqref="H2:H25">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I24">
+  <conditionalFormatting sqref="I2:I25">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1862,7 +1914,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1942,6 +1994,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:04:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1865,8 +1865,59 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Ik heb geen orderbevestiging gekregen</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Testmail #11: Ik heb geen orderbevestiging gekregen</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor het melden van dit probleem. Om u beter van dienst te kunnen zijn, zou u ons uw bestelnummer of de datum van uw bestelling kunnen doorgeven? Hiermee kunnen we nagaan wat er mogelijk is misgegaan met de orderbevestiging.
+We doen ons best om dit zo snel mogelijk voor u op te lossen. Alvast bedankt voor uw medewerking!
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:04:32</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1886,7 +1937,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1894,12 +1945,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H25">
+  <conditionalFormatting sqref="H2:H26">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I25">
+  <conditionalFormatting sqref="I2:I26">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1941,7 +1992,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$8</f>
+              <f>'Dashboard'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$8</f>
+              <f>'Dashboard'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1916,8 +1916,58 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Wanneer komt mijn offerte?</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Testmail #12: Wanneer komt mijn offerte?</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u voor uw e-mail. Uw offerte zal naar verwachting binnen 24 uur worden verstuurd. Mocht u deze niet op tijd ontvangen, neem dan gerust contact met ons op.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:06:42</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1937,7 +1987,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1945,12 +1995,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26">
+  <conditionalFormatting sqref="H2:H27">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I26">
+  <conditionalFormatting sqref="I2:I27">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1965,7 +2015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2055,6 +2105,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:09:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1966,8 +1966,58 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Zijn jullie telefonisch bereikbaar?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Testmail #13: Zijn jullie telefonisch bereikbaar?</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw e-mail. Op dit moment zijn wij helaas niet telefonisch bereikbaar. Als u vragen heeft of hulp nodig heeft, kunt u ons altijd per e-mail bereiken op dit adres. We streven ernaar om binnen 24 uur te reageren op alle vragen en verzoeken die we ontvangen.
+Met vriendelijke groet,
+[Naam van het bedrijf] assistent</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:08:52</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1987,7 +2037,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1995,12 +2045,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H27">
+  <conditionalFormatting sqref="H2:H28">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I27">
+  <conditionalFormatting sqref="I2:I28">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2048,7 +2098,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2058,11 +2108,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2016,8 +2016,58 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Kun je deze bestelling vandaag verwerken?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Testmail #14: Kun je deze bestelling vandaag verwerken?</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Hartelijk dank voor uw e-mail. Om de bestelling vandaag te kunnen verwerken, hebben we een ordernummer of klantgegevens nodig. Zou u ons deze gegevens kunnen verstrekken, zodat we uw verzoek verder kunnen onderzoeken?
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:11:04</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2037,7 +2087,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2045,12 +2095,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H28">
+  <conditionalFormatting sqref="H2:H29">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I28">
+  <conditionalFormatting sqref="I2:I29">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2092,7 +2142,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:13:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2066,8 +2066,59 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Ik wil mijn gegevens aanpassen</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Testmail #15: Ik wil mijn gegevens aanpassen</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u voor uw bericht. Om uw gegevens aan te passen, kunt u inloggen op onze website met uw gebruikersnaam en wachtwoord. Eenmaal ingelogd, kunt u uw persoonlijke gegevens bijwerken onder uw accountinstellingen.
+Mocht u nog verdere assistentie nodig hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:13:14</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2087,7 +2138,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2095,12 +2146,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H29">
+  <conditionalFormatting sqref="H2:H30">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I29">
+  <conditionalFormatting sqref="I2:I30">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2182,7 +2233,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2117,8 +2117,58 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Kun je dit product voor mij bestellen?</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Testmail #16: Kun je dit product voor mij bestellen?</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u wel voor uw interesse in ons product. Helaas kunnen wij op basis van deze e-mail geen bestelling voor u plaatsen. U kunt echter onze website bezoeken en het product zelf bestellen. Mocht u verdere vragen hebben of hulp nodig hebben bij het plaatsen van een bestelling, dan helpen wij u graag verder.
+Met vriendelijke groet,
+[Naam Bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:15:43</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D31">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2138,7 +2188,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2146,12 +2196,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H30">
+  <conditionalFormatting sqref="H2:H31">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I30">
+  <conditionalFormatting sqref="I2:I31">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2193,7 +2243,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:18:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2167,8 +2167,59 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Ik heb een klacht</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Testmail #17: Ik heb een klacht</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor het doorsturen van uw klacht. Om uw klacht zo goed mogelijk te kunnen behandelen, ontvangen wij graag meer informatie over de aard van de klacht. Kunt u ons meer details geven over wat er precies is misgegaan? 
+Met vriendelijke groet,
+[Naam] 
+Klantenservice Team</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:17:57</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D31">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2188,7 +2239,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G31">
+  <conditionalFormatting sqref="G2:G32">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2196,12 +2247,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H31">
+  <conditionalFormatting sqref="H2:H32">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I31">
+  <conditionalFormatting sqref="I2:I32">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2293,7 +2344,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:20:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$9</f>
+              <f>'Dashboard'!$A$2:$A$10</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$9</f>
+              <f>'Dashboard'!$B$2:$B$10</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2218,8 +2218,59 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Ik wil een afspraak plannen, regel jij dat?</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Testmail #18: Ik wil een afspraak plannen, regel jij dat?</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je e-mail. Helaas kan ik geen afspraken plannen via e-mail. Graag verzoek ik je om contact op te nemen met onze klantenservice of receptie om een afspraak te maken. Je kunt ons bereiken via [telefoonnummer] of [e-mailadres]. Onze medewerkers staan klaar om je verder te helpen.
+Met vriendelijke groet,
+[Naam] 
+E-mailassistent bij [Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:20:11</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2239,7 +2290,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G32">
+  <conditionalFormatting sqref="G2:G33">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2247,12 +2298,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H32">
+  <conditionalFormatting sqref="H2:H33">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I32">
+  <conditionalFormatting sqref="I2:I33">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2267,7 +2318,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2367,6 +2418,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:22:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -225,12 +225,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$10</f>
+              <f>'Dashboard'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$10</f>
+              <f>'Dashboard'!$B$2:$B$11</f>
             </numRef>
           </val>
         </ser>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2269,8 +2269,58 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Zijn er vacatures?</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Testmail #19: Zijn er vacatures?</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Beste,
+Dank u voor uw interesse in onze organisatie. Op dit moment hebben we geen openstaande vacatures, maar we moedigen u aan om regelmatig onze website te bezoeken voor eventuele toekomstige mogelijkheden. Mocht u nog vragen hebben of meer informatie wensen, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:22:21</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D33">
+  <conditionalFormatting sqref="D2:D34">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2290,7 +2340,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G33">
+  <conditionalFormatting sqref="G2:G34">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2298,12 +2348,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H33">
+  <conditionalFormatting sqref="H2:H34">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I33">
+  <conditionalFormatting sqref="I2:I34">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2318,7 +2368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2428,6 +2478,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-29 15:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-29.xlsx
+++ b/logs/mail_log_2025-06-29.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2319,8 +2319,59 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Kun je deze taak op je nemen?</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Testmail #20: Kun je deze taak op je nemen?</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Bedankt voor je bericht. Kun je wat meer details geven over welke taak je precies bedoelt? Dan kan ik je zo goed mogelijk helpen.
+Met vriendelijke groet,
+[Jouw naam]  
+E-mailassistent bij [Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-06-29 15:24:39</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D34">
+  <conditionalFormatting sqref="D2:D35">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2340,7 +2391,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G34">
+  <conditionalFormatting sqref="G2:G35">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2348,12 +2399,12 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H34">
+  <conditionalFormatting sqref="H2:H35">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I34">
+  <conditionalFormatting sqref="I2:I35">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2421,17 +2472,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Retour / Terugbetaling</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Retour / Terugbetaling</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>